<commit_message>
added a refs stats dashboard
</commit_message>
<xml_diff>
--- a/refs_finish_stats_dshb.xlsx
+++ b/refs_finish_stats_dshb.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="29">
   <si>
     <t>ref</t>
   </si>
@@ -2523,6 +2523,141 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="24"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="25"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="26"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="28"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -2555,63 +2690,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2619,7 +2698,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2631,7 +2710,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.1250000000000002E-3</c:v>
+                  <c:v>2.8901734104046237E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2667,63 +2746,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2731,7 +2754,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2743,7 +2766,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.40625E-2</c:v>
+                  <c:v>1.4450867052023118E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2779,63 +2802,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2843,7 +2810,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2855,7 +2822,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.9374999999999997E-2</c:v>
+                  <c:v>0.10982658959537568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2891,63 +2858,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2955,7 +2866,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2967,7 +2878,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.2578125</c:v>
+                  <c:v>0.37572254335260108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2987,7 +2898,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DQ</c:v>
+                  <c:v>KO/TKO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3011,7 +2922,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3023,7 +2934,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5625000000000001E-3</c:v>
+                  <c:v>0.31791907514450868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3043,7 +2954,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KO/TKO</c:v>
+                  <c:v>Overturned</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3059,63 +2970,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3123,7 +2978,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3135,7 +2990,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.359375</c:v>
+                  <c:v>2.8901734104046237E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3155,7 +3010,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Other</c:v>
+                  <c:v>Submission</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3173,63 +3028,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3237,7 +3036,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3249,7 +3048,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.1250000000000002E-3</c:v>
+                  <c:v>0.17341040462427745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3269,7 +3068,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Overturned</c:v>
+                  <c:v>TKO - Doctor's Stoppage</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3287,63 +3086,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3351,7 +3094,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3363,7 +3106,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5625E-2</c:v>
+                  <c:v>2.8901734104046237E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3371,234 +3114,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-73B1-4723-ACAD-B5FFCAE30AD7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pivot!$J$34:$J$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Submission</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pivot!$A$36:$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pivot!$J$36:$J$37</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.2578125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-73B1-4723-ACAD-B5FFCAE30AD7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pivot!$K$34:$K$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TKO - Doctor's Stoppage</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pivot!$A$36:$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pivot!$K$36:$K$37</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.8125000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-73B1-4723-ACAD-B5FFCAE30AD7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3958,7 +3473,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3966,19 +3481,16 @@
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="cs-CZ" sz="1800"/>
-              <a:t>Fight Outcomes</a:t>
+              <a:rPr lang="cs-CZ" sz="2400">
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Fight Outcomes by Finish Type</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="cs-CZ" sz="1800" baseline="0"/>
-              <a:t> by Finish Type</a:t>
-            </a:r>
-            <a:endParaRPr lang="cs-CZ" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3996,7 +3508,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4004,8 +3516,8 @@
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="cs-CZ"/>
@@ -4016,199 +3528,38 @@
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="3"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="4"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="5"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="6"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="7"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="8"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="9"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="10"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4223,49 +3574,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="11"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4280,49 +3590,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="12"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4337,49 +3606,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="13"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4394,64 +3622,11 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="14"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="15"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4466,64 +3641,11 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="16"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="17"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4538,49 +3660,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="18"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4595,49 +3676,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="19"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4652,49 +3692,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="20"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4709,49 +3708,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="21"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4766,49 +3724,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="22"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4823,49 +3740,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="23"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4880,49 +3756,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="24"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4937,49 +3772,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="25"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -4994,49 +3788,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="26"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5051,49 +3804,8 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="27"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5108,50 +3820,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="28"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5168,50 +3839,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="29"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5228,50 +3858,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="30"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5288,50 +3877,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="31"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5348,50 +3896,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="32"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5408,50 +3915,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="33"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5468,50 +3934,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="34"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5528,50 +3953,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="35"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5587,126 +3971,10 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="36"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="37"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="38"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="39"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="40"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
         <c:idx val="41"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5723,50 +3991,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="42"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5783,50 +4010,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="43"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5842,66 +4028,10 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="44"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
         <c:idx val="45"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="cs-CZ"/>
-            </a:p>
-          </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -5915,6 +4045,122 @@
             </c:ext>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="46"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="70000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="47"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="70000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="48"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="70000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="49"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="70000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -5949,7 +4195,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -5966,7 +4214,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5978,7 +4226,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.1250000000000002E-3</c:v>
+                  <c:v>2.8901734104046237E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6005,7 +4253,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent2">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6022,7 +4272,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6034,7 +4284,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.40625E-2</c:v>
+                  <c:v>1.4450867052023118E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6061,7 +4311,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent3">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6078,7 +4330,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6090,7 +4342,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.9374999999999997E-2</c:v>
+                  <c:v>0.10982658959537568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6117,7 +4369,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent4">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6134,7 +4388,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6146,7 +4400,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.2578125</c:v>
+                  <c:v>0.37572254335260108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6166,14 +4420,16 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DQ</c:v>
+                  <c:v>KO/TKO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:schemeClr val="accent5">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6190,7 +4446,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6202,7 +4458,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5625000000000001E-3</c:v>
+                  <c:v>0.31791907514450868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6222,14 +4478,16 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KO/TKO</c:v>
+                  <c:v>Overturned</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="accent6">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6246,7 +4504,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6258,7 +4516,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.359375</c:v>
+                  <c:v>2.8901734104046237E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6278,7 +4536,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Other</c:v>
+                  <c:v>Submission</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6287,6 +4545,7 @@
             <a:solidFill>
               <a:schemeClr val="accent1">
                 <a:lumMod val="60000"/>
+                <a:alpha val="70000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -6296,63 +4555,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -6360,7 +4563,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6372,7 +4575,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.1250000000000002E-3</c:v>
+                  <c:v>0.17341040462427745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6392,7 +4595,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Overturned</c:v>
+                  <c:v>TKO - Doctor's Stoppage</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6401,6 +4604,7 @@
             <a:solidFill>
               <a:schemeClr val="accent2">
                 <a:lumMod val="60000"/>
+                <a:alpha val="70000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -6410,63 +4614,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -6474,7 +4622,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
+                  <c:v>Marc Goddard</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6486,7 +4634,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5625E-2</c:v>
+                  <c:v>2.8901734104046237E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6494,234 +4642,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-7A93-4457-8E3B-88CBE4E36BDE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pivot!$J$34:$J$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Submission</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pivot!$A$36:$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pivot!$J$36:$J$37</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.2578125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-7A93-4457-8E3B-88CBE4E36BDE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pivot!$K$34:$K$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TKO - Doctor's Stoppage</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="cs-CZ"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pivot!$A$36:$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>John McCarthy</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pivot!$K$36:$K$37</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.8125000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-7A93-4457-8E3B-88CBE4E36BDE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6734,8 +4654,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
         <c:axId val="1051821696"/>
         <c:axId val="1051824192"/>
       </c:barChart>
@@ -6753,7 +4673,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6786,7 +4706,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6808,11 +4728,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -6824,7 +4744,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6858,8 +4778,8 @@
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -6874,7 +4794,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6888,13 +4808,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="cs-CZ"/>
-                  <a:t>Percentages</a:t>
+                  <a:t>Percentages of Fight Outcomes</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="cs-CZ" baseline="0"/>
-                  <a:t> of Fight Outcomes</a:t>
-                </a:r>
-                <a:endParaRPr lang="cs-CZ"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6912,7 +4827,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6944,7 +4859,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7018,7 +4933,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -10080,7 +7995,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -10091,7 +8006,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -10104,6 +8019,29 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -10115,29 +8053,6 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -10156,23 +8071,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="bg1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -10181,70 +8088,84 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -10266,15 +8187,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -10289,8 +8208,8 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
@@ -10308,10 +8227,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -10327,10 +8246,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -10346,40 +8265,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -10392,20 +8286,38 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:gridlineMinor>
   <cs:hiLoLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -10417,17 +8329,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -10441,14 +8352,14 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -10456,7 +8367,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -10476,10 +8387,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -10494,13 +8405,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:fontRef idx="major">
       <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -10509,14 +8420,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="15875" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -10546,8 +8456,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -10563,21 +8473,15 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -11628,7 +9532,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
+      <xdr:colOff>83820</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>112395</xdr:rowOff>
     </xdr:to>
@@ -13461,17 +11365,17 @@
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Kontingenční tabulka2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A34:L37" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A34:J37" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
       <items count="11">
         <item h="1" x="2"/>
         <item h="1" x="0"/>
         <item h="1" x="9"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item h="1" x="8"/>
         <item h="1" x="7"/>
-        <item h="1" x="4"/>
+        <item x="4"/>
         <item h="1" x="3"/>
         <item h="1" x="6"/>
         <item h="1" x="5"/>
@@ -13501,7 +11405,7 @@
   </rowFields>
   <rowItems count="2">
     <i>
-      <x v="3"/>
+      <x v="6"/>
     </i>
     <i t="grand">
       <x/>
@@ -13510,7 +11414,7 @@
   <colFields count="1">
     <field x="1"/>
   </colFields>
-  <colItems count="11">
+  <colItems count="9">
     <i>
       <x/>
     </i>
@@ -13524,13 +11428,7 @@
       <x v="3"/>
     </i>
     <i>
-      <x v="4"/>
-    </i>
-    <i>
       <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
     </i>
     <i>
       <x v="7"/>
@@ -13548,8 +11446,56 @@
   <dataFields count="1">
     <dataField name="Součet z percentage" fld="3" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
-  <chartFormats count="20">
-    <chartFormat chart="0" format="10" series="1">
+  <chartFormats count="19">
+    <chartFormat chart="2" format="46" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="47" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="48" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="49" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="50" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13561,7 +11507,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="11" series="1">
+    <chartFormat chart="2" format="51" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13573,7 +11519,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="12" series="1">
+    <chartFormat chart="2" format="52" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13585,7 +11531,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="13" series="1">
+    <chartFormat chart="2" format="53" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13597,7 +11543,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="14" series="1">
+    <chartFormat chart="2" format="54" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13609,7 +11555,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="15" series="1">
+    <chartFormat chart="2" format="55" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13621,19 +11567,67 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="16" series="1">
+    <chartFormat chart="0" format="20" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
-            <x v="6"/>
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="17" series="1">
+    <chartFormat chart="0" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="23" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="24" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="25" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13645,7 +11639,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="18" series="1">
+    <chartFormat chart="0" format="26" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13657,7 +11651,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="19" series="1">
+    <chartFormat chart="0" format="27" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13669,7 +11663,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="36" series="1">
+    <chartFormat chart="0" format="28" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13677,114 +11671,6 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="37" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="38" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="39" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="40" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="41" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="42" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="43" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="44" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="45" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -13810,10 +11696,10 @@
         <i x="2"/>
         <i x="0"/>
         <i x="9"/>
-        <i x="1" s="1"/>
+        <i x="1"/>
         <i x="8"/>
         <i x="7"/>
-        <i x="4"/>
+        <i x="4" s="1"/>
         <i x="3"/>
         <i x="6"/>
         <i x="5"/>
@@ -15233,7 +13119,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
@@ -15242,14 +13128,15 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" customWidth="1"/>
     <col min="11" max="11" width="21.6640625" customWidth="1"/>
     <col min="12" max="12" width="13.77734375" customWidth="1"/>
     <col min="13" max="18" width="12" customWidth="1"/>
@@ -15736,7 +13623,7 @@
         <v>988.79211180473078</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
@@ -15744,7 +13631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
@@ -15761,100 +13648,82 @@
         <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J35" t="s">
-        <v>11</v>
-      </c>
-      <c r="K35" t="s">
-        <v>12</v>
-      </c>
-      <c r="L35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B36" s="5">
-        <v>3.1250000000000002E-3</v>
+        <v>2.8901734104046237E-3</v>
       </c>
       <c r="C36" s="5">
-        <v>1.40625E-2</v>
+        <v>1.4450867052023118E-2</v>
       </c>
       <c r="D36" s="5">
-        <v>5.9374999999999997E-2</v>
+        <v>0.10982658959537568</v>
       </c>
       <c r="E36" s="5">
-        <v>0.2578125</v>
+        <v>0.37572254335260108</v>
       </c>
       <c r="F36" s="5">
-        <v>1.5625000000000001E-3</v>
+        <v>0.31791907514450868</v>
       </c>
       <c r="G36" s="5">
-        <v>0.359375</v>
+        <v>2.8901734104046237E-3</v>
       </c>
       <c r="H36" s="5">
-        <v>3.1250000000000002E-3</v>
+        <v>0.17341040462427745</v>
       </c>
       <c r="I36" s="5">
-        <v>1.5625E-2</v>
+        <v>2.8901734104046237E-3</v>
       </c>
       <c r="J36" s="5">
-        <v>0.2578125</v>
-      </c>
-      <c r="K36" s="5">
-        <v>2.8125000000000001E-2</v>
-      </c>
-      <c r="L36" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B37" s="5">
-        <v>3.1250000000000002E-3</v>
+        <v>2.8901734104046237E-3</v>
       </c>
       <c r="C37" s="5">
-        <v>1.40625E-2</v>
+        <v>1.4450867052023118E-2</v>
       </c>
       <c r="D37" s="5">
-        <v>5.9374999999999997E-2</v>
+        <v>0.10982658959537568</v>
       </c>
       <c r="E37" s="5">
-        <v>0.2578125</v>
+        <v>0.37572254335260108</v>
       </c>
       <c r="F37" s="5">
-        <v>1.5625000000000001E-3</v>
+        <v>0.31791907514450868</v>
       </c>
       <c r="G37" s="5">
-        <v>0.359375</v>
+        <v>2.8901734104046237E-3</v>
       </c>
       <c r="H37" s="5">
-        <v>3.1250000000000002E-3</v>
+        <v>0.17341040462427745</v>
       </c>
       <c r="I37" s="5">
-        <v>1.5625E-2</v>
+        <v>2.8901734104046237E-3</v>
       </c>
       <c r="J37" s="5">
-        <v>0.2578125</v>
-      </c>
-      <c r="K37" s="5">
-        <v>2.8125000000000001E-2</v>
-      </c>
-      <c r="L37" s="5">
         <v>1</v>
       </c>
     </row>
@@ -16983,7 +14852,7 @@
   <dimension ref="A2:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>